<commit_message>
Testing with new parameters
</commit_message>
<xml_diff>
--- a/data/testing/PyNeapple_test_results.xlsx
+++ b/data/testing/PyNeapple_test_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonas\Desktop\Pyneapple\data\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{575D8FE3-F6CB-4C78-8FB2-D2B8E765EFAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7DF39CE-B535-4B1A-BABA-B57C41B84DDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16457" windowHeight="17914" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="relativ" sheetId="4" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="21">
   <si>
     <t>NNLS</t>
   </si>
@@ -83,6 +83,12 @@
   </si>
   <si>
     <t>0.2</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>reg = 0*</t>
   </si>
 </sst>
 </file>
@@ -487,7 +493,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD789FA1-9799-4583-AE09-28D4F507798E}">
   <dimension ref="A1:N36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
@@ -586,19 +592,19 @@
       </c>
       <c r="D4" s="4">
         <f>$L$4/absolut!D4*100</f>
-        <v>81.101594935070523</v>
+        <v>67.604874451928978</v>
       </c>
       <c r="E4" s="4">
         <f>$M$4/absolut!E4*100</f>
-        <v>75.667058979682579</v>
+        <v>57.939015352312218</v>
       </c>
       <c r="F4" s="4">
         <f>$L$4/absolut!F4*100</f>
-        <v>113.46398420478178</v>
+        <v>104.35622380550677</v>
       </c>
       <c r="G4" s="4">
         <f>$M$4/absolut!G4*100</f>
-        <v>127.87434170772541</v>
+        <v>113.19130228106017</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="4">
@@ -626,19 +632,19 @@
       </c>
       <c r="D5" s="4">
         <f>$L$5/absolut!D5*100</f>
-        <v>94.588881638212897</v>
+        <v>84.935811597327955</v>
       </c>
       <c r="E5" s="4">
         <f>$M$5/absolut!E5*100</f>
-        <v>115.85934888769491</v>
+        <v>136.41187640875862</v>
       </c>
       <c r="F5" s="4">
         <f>$L$5/absolut!F5*100</f>
-        <v>106.87316843447367</v>
+        <v>105.63206522262176</v>
       </c>
       <c r="G5" s="4">
         <f>$M$5/absolut!G5*100</f>
-        <v>85.678788217260688</v>
+        <v>84.136707720467498</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="4">
@@ -666,19 +672,19 @@
       </c>
       <c r="D6" s="4">
         <f>$L$6/absolut!D6*100</f>
-        <v>208.05184231032149</v>
+        <v>153.42855792946946</v>
       </c>
       <c r="E6" s="4">
         <f>$M$6/absolut!E6*100</f>
-        <v>99.154145599124291</v>
+        <v>104.42808276417179</v>
       </c>
       <c r="F6" s="4">
         <f>$L$6/absolut!F6*100</f>
-        <v>162.97251859418012</v>
+        <v>138.24725612545851</v>
       </c>
       <c r="G6" s="4">
         <f>$M$6/absolut!G6*100</f>
-        <v>91.926221397608685</v>
+        <v>98.117995086244918</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="4">
@@ -734,19 +740,19 @@
       </c>
       <c r="D8" s="4">
         <f>$L$4/absolut!D8*100</f>
-        <v>215.40617528952239</v>
+        <v>67.604874451928978</v>
       </c>
       <c r="E8" s="4">
         <f>$M$4/absolut!E8*100</f>
-        <v>233.41779543398204</v>
+        <v>57.939015352312218</v>
       </c>
       <c r="F8" s="4">
         <f>$L$4/absolut!F8*100</f>
-        <v>113.46398420478178</v>
+        <v>104.35622380550677</v>
       </c>
       <c r="G8" s="4">
         <f>$M$4/absolut!G8*100</f>
-        <v>127.87434170772541</v>
+        <v>113.19130228106017</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
@@ -764,19 +770,19 @@
       </c>
       <c r="D9" s="4">
         <f>$L$5/absolut!D9*100</f>
-        <v>117.1224451993355</v>
+        <v>84.935811597327955</v>
       </c>
       <c r="E9" s="4">
         <f>$M$5/absolut!E9*100</f>
-        <v>95.78797078513746</v>
+        <v>136.41187640875862</v>
       </c>
       <c r="F9" s="4">
         <f>$L$5/absolut!F9*100</f>
-        <v>106.87316843447367</v>
+        <v>105.63206522262176</v>
       </c>
       <c r="G9" s="4">
         <f>$M$5/absolut!G9*100</f>
-        <v>85.678788217260688</v>
+        <v>84.136707720467498</v>
       </c>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
@@ -794,19 +800,19 @@
       </c>
       <c r="D10" s="4">
         <f>$L$6/absolut!D10*100</f>
-        <v>527.79347146861744</v>
+        <v>153.42855792946946</v>
       </c>
       <c r="E10" s="4">
         <f>$M$6/absolut!E10*100</f>
-        <v>78.54911883863042</v>
+        <v>104.42808276417179</v>
       </c>
       <c r="F10" s="4">
         <f>$L$6/absolut!F10*100</f>
-        <v>162.97251859418012</v>
+        <v>138.24725612545851</v>
       </c>
       <c r="G10" s="4">
         <f>$M$6/absolut!G10*100</f>
-        <v>91.926221397608685</v>
+        <v>98.117995086244918</v>
       </c>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
@@ -875,19 +881,19 @@
       </c>
       <c r="D13" s="4">
         <f>$L$4/absolut!D13*100</f>
-        <v>1429.5566210454394</v>
+        <v>236.03380303131573</v>
       </c>
       <c r="E13" s="4">
         <f>$M$4/absolut!E13*100</f>
-        <v>373.8937153072057</v>
+        <v>170.17883467533602</v>
       </c>
       <c r="F13" s="4">
         <f>$L$4/absolut!F13*100</f>
-        <v>1473.8677290329415</v>
+        <v>236.03380303131573</v>
       </c>
       <c r="G13" s="4">
         <f>$M$4/absolut!G13*100</f>
-        <v>400.66893943713904</v>
+        <v>172.09790475997926</v>
       </c>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
@@ -905,19 +911,19 @@
       </c>
       <c r="D14" s="4">
         <f>$L$5/absolut!D14*100</f>
-        <v>120.75281928916522</v>
+        <v>112.13899555432947</v>
       </c>
       <c r="E14" s="4">
         <f>$M$5/absolut!E14*100</f>
-        <v>90.375301296345071</v>
+        <v>99.10757542477036</v>
       </c>
       <c r="F14" s="4">
         <f>$L$5/absolut!F14*100</f>
-        <v>120.75281928916523</v>
+        <v>114.08593207229161</v>
       </c>
       <c r="G14" s="4">
         <f>$M$5/absolut!G14*100</f>
-        <v>89.050885398246606</v>
+        <v>98.152895192211503</v>
       </c>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
@@ -935,19 +941,19 @@
       </c>
       <c r="D15" s="4">
         <f>$L$6/absolut!D15*100</f>
-        <v>120.09996793759153</v>
+        <v>75.283540887464667</v>
       </c>
       <c r="E15" s="4">
         <f>$M$6/absolut!E15*100</f>
-        <v>50.731211468047199</v>
+        <v>53.606067337368614</v>
       </c>
       <c r="F15" s="4">
         <f>$L$6/absolut!F15*100</f>
-        <v>120.09996793759159</v>
+        <v>75.283540887464667</v>
       </c>
       <c r="G15" s="4">
         <f>$M$6/absolut!G15*100</f>
-        <v>49.540020833944723</v>
+        <v>54.045243711550839</v>
       </c>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
@@ -1085,19 +1091,19 @@
       </c>
       <c r="D22" s="4">
         <f>$L$22/absolut!D22*100</f>
-        <v>84.366681202734298</v>
+        <v>62.073251892177595</v>
       </c>
       <c r="E22" s="4">
         <f>$M$22/absolut!E22*100</f>
-        <v>87.355031009956335</v>
+        <v>85.41746337299378</v>
       </c>
       <c r="F22" s="4">
         <f>$L$22/absolut!F22*100</f>
-        <v>86.981744549149752</v>
+        <v>89.387828586157923</v>
       </c>
       <c r="G22" s="4">
         <f>$M$22/absolut!G22*100</f>
-        <v>88.046554528637557</v>
+        <v>95.837947425229146</v>
       </c>
       <c r="H22" s="1"/>
       <c r="I22" s="4">
@@ -1125,19 +1131,19 @@
       </c>
       <c r="D23" s="4">
         <f>$L$23/absolut!D23*100</f>
-        <v>83.589254050328137</v>
+        <v>62.26866104106611</v>
       </c>
       <c r="E23" s="4">
         <f>$M$23/absolut!E23*100</f>
-        <v>116.950417168321</v>
+        <v>133.06582392281351</v>
       </c>
       <c r="F23" s="4">
         <f>$L$23/absolut!F23*100</f>
-        <v>86.180219954225066</v>
+        <v>99.516043141069176</v>
       </c>
       <c r="G23" s="4">
         <f>$M$23/absolut!G23*100</f>
-        <v>105.07756731434617</v>
+        <v>75.48289862796473</v>
       </c>
       <c r="H23" s="1"/>
       <c r="I23" s="4">
@@ -1165,19 +1171,19 @@
       </c>
       <c r="D24" s="4">
         <f>$L$24/absolut!D24*100</f>
-        <v>126.48936974315134</v>
+        <v>110.16084062728955</v>
       </c>
       <c r="E24" s="4">
         <f>$M$24/absolut!E24*100</f>
-        <v>107.76359808461082</v>
+        <v>101.71965262045457</v>
       </c>
       <c r="F24" s="4">
         <f>$L$24/absolut!F24*100</f>
-        <v>118.99801896353675</v>
+        <v>108.26438856892192</v>
       </c>
       <c r="G24" s="4">
         <f>$M$24/absolut!G24*100</f>
-        <v>96.417772962499001</v>
+        <v>83.276805327724603</v>
       </c>
       <c r="H24" s="1"/>
       <c r="I24" s="4">
@@ -1233,19 +1239,19 @@
       </c>
       <c r="D26" s="4">
         <f>$L$22/absolut!D26*100</f>
-        <v>146.15027593477342</v>
+        <v>62.073251892177595</v>
       </c>
       <c r="E26" s="4">
         <f>$M$22/absolut!E26*100</f>
-        <v>127.06207890948427</v>
+        <v>85.41746337299378</v>
       </c>
       <c r="F26" s="4">
         <f>$L$22/absolut!F26*100</f>
-        <v>86.981744549149752</v>
+        <v>89.387828586157923</v>
       </c>
       <c r="G26" s="4">
         <f>$M$22/absolut!G26*100</f>
-        <v>88.046554528637557</v>
+        <v>95.837947425229146</v>
       </c>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
@@ -1263,19 +1269,19 @@
       </c>
       <c r="D27" s="4">
         <f>$L$23/absolut!D27*100</f>
-        <v>144.80352160920856</v>
+        <v>62.26866104106611</v>
       </c>
       <c r="E27" s="4">
         <f>$M$23/absolut!E27*100</f>
-        <v>68.803269242169179</v>
+        <v>133.06582392281351</v>
       </c>
       <c r="F27" s="4">
         <f>$L$23/absolut!F27*100</f>
-        <v>86.180219954225066</v>
+        <v>99.516043141069176</v>
       </c>
       <c r="G27" s="4">
         <f>$M$23/absolut!G27*100</f>
-        <v>105.07756731434617</v>
+        <v>75.48289862796473</v>
       </c>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
@@ -1293,19 +1299,19 @@
       </c>
       <c r="D28" s="4">
         <f>$L$24/absolut!D28*100</f>
-        <v>306.55707058239147</v>
+        <v>110.16084062728955</v>
       </c>
       <c r="E28" s="4">
         <f>$M$24/absolut!E28*100</f>
-        <v>108.47157912507137</v>
+        <v>101.71965262045457</v>
       </c>
       <c r="F28" s="4">
         <f>$L$24/absolut!F28*100</f>
-        <v>118.99801896353675</v>
+        <v>108.26438856892192</v>
       </c>
       <c r="G28" s="4">
         <f>$M$24/absolut!G28*100</f>
-        <v>96.417772962499001</v>
+        <v>83.276805327724603</v>
       </c>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
@@ -1397,19 +1403,19 @@
       </c>
       <c r="D32" s="4">
         <f>$L$22/absolut!D32*100</f>
-        <v>412.61279507547846</v>
+        <v>113.98848475665757</v>
       </c>
       <c r="E32" s="4">
         <f>$M$22/absolut!E32*100</f>
-        <v>216.68028713495778</v>
+        <v>101.78570051557773</v>
       </c>
       <c r="F32" s="4">
         <f>$L$22/absolut!F32*100</f>
-        <v>92.457556377917811</v>
+        <v>113.9884847566576</v>
       </c>
       <c r="G32" s="4">
         <f>$M$22/absolut!G32*100</f>
-        <v>116.61399482246804</v>
+        <v>101.76091175074467</v>
       </c>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
@@ -1427,19 +1433,19 @@
       </c>
       <c r="D33" s="4">
         <f>$L$23/absolut!D33*100</f>
-        <v>179.29953532185255</v>
+        <v>114.34732519292281</v>
       </c>
       <c r="E33" s="4">
         <f>$M$23/absolut!E33*100</f>
-        <v>57.59514853990332</v>
+        <v>103.7120637650754</v>
       </c>
       <c r="F33" s="4">
         <f>$L$23/absolut!F33*100</f>
-        <v>136.22751259990753</v>
+        <v>114.34732519292281</v>
       </c>
       <c r="G33" s="4">
         <f>$M$23/absolut!G33*100</f>
-        <v>78.060768878904781</v>
+        <v>103.7120637650754</v>
       </c>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
@@ -1457,19 +1463,19 @@
       </c>
       <c r="D34" s="4">
         <f>$L$24/absolut!D34*100</f>
-        <v>105.32006953480601</v>
+        <v>76.498576115660072</v>
       </c>
       <c r="E34" s="4">
         <f>$M$24/absolut!E34*100</f>
-        <v>50.114270949510519</v>
+        <v>86.119692474224181</v>
       </c>
       <c r="F34" s="4">
         <f>$L$24/absolut!F34*100</f>
-        <v>105.32006953480601</v>
+        <v>76.498576115660072</v>
       </c>
       <c r="G34" s="4">
         <f>$M$24/absolut!G34*100</f>
-        <v>49.398749892913244</v>
+        <v>85.570084642316303</v>
       </c>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
@@ -1528,10 +1534,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BB2ACD8-0A1F-4239-A3F7-5D8380960D13}">
-  <dimension ref="A1:N36"/>
+  <dimension ref="A1:Q36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1628,16 +1634,16 @@
         <v>1</v>
       </c>
       <c r="D4">
-        <v>2.4660427474961361E-3</v>
+        <v>2.9583665618994931E-3</v>
       </c>
       <c r="E4">
-        <v>0.33039476275551782</v>
+        <v>0.4314881750747997</v>
       </c>
       <c r="F4">
-        <v>1.7626738687320949E-3</v>
+        <v>1.9165124293185299E-3</v>
       </c>
       <c r="G4">
-        <v>0.19550442775409141</v>
+        <v>0.22086502669545791</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4">
@@ -1662,16 +1668,16 @@
         <v>2</v>
       </c>
       <c r="D5">
-        <v>7.400446943409124E-3</v>
+        <v>8.2415177630682911E-3</v>
       </c>
       <c r="E5">
-        <v>0.64733662600416642</v>
+        <v>0.54980550062417044</v>
       </c>
       <c r="F5">
-        <v>6.549819849583533E-3</v>
+        <v>6.626775671996335E-3</v>
       </c>
       <c r="G5">
-        <v>0.87536252041541651</v>
+        <v>0.89140640312641017</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5">
@@ -1696,16 +1702,16 @@
         <v>3</v>
       </c>
       <c r="D6">
-        <v>9.6129886560527691E-2</v>
+        <v>0.130353828973573</v>
       </c>
       <c r="E6">
-        <v>5.0426535066065453E-2</v>
+        <v>4.7879841012607859E-2</v>
       </c>
       <c r="F6">
-        <v>0.122720076811246</v>
+        <v>0.14466833238158541</v>
       </c>
       <c r="G6">
-        <v>5.4391444834586307E-2</v>
+        <v>5.0959051860008361E-2</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6">
@@ -1730,10 +1736,10 @@
         <v>4</v>
       </c>
       <c r="D7">
-        <v>0.15195523218213769</v>
+        <v>0.1910026074596459</v>
       </c>
       <c r="E7">
-        <v>3.8077307906776041E-2</v>
+        <v>3.475941023606554E-2</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
@@ -1752,16 +1758,16 @@
         <v>1</v>
       </c>
       <c r="D8">
-        <v>9.284784882846775E-4</v>
+        <v>2.9583665618994931E-3</v>
       </c>
       <c r="E8">
-        <v>0.10710408755904299</v>
+        <v>0.4314881750747997</v>
       </c>
       <c r="F8">
-        <v>1.7626738687320949E-3</v>
+        <v>1.9165124293185299E-3</v>
       </c>
       <c r="G8">
-        <v>0.19550442775409141</v>
+        <v>0.22086502669545791</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
@@ -1778,16 +1784,16 @@
         <v>2</v>
       </c>
       <c r="D9">
-        <v>5.9766511773950868E-3</v>
+        <v>8.2415177630682911E-3</v>
       </c>
       <c r="E9">
-        <v>0.78297931760380357</v>
+        <v>0.54980550062417044</v>
       </c>
       <c r="F9">
-        <v>6.549819849583533E-3</v>
+        <v>6.626775671996335E-3</v>
       </c>
       <c r="G9">
-        <v>0.87536252041541651</v>
+        <v>0.89140640312641017</v>
       </c>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
@@ -1804,16 +1810,16 @@
         <v>3</v>
       </c>
       <c r="D10">
-        <v>3.7893610059913749E-2</v>
+        <v>0.130353828973573</v>
       </c>
       <c r="E10">
-        <v>6.3654437808168041E-2</v>
+        <v>4.7879841012607859E-2</v>
       </c>
       <c r="F10">
-        <v>0.122720076811246</v>
+        <v>0.14466833238158541</v>
       </c>
       <c r="G10">
-        <v>5.4391444834586307E-2</v>
+        <v>5.0959051860008361E-2</v>
       </c>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
@@ -1830,10 +1836,10 @@
         <v>4</v>
       </c>
       <c r="D11">
-        <v>0.138657770471422</v>
+        <v>0.1910026074596459</v>
       </c>
       <c r="E11">
-        <v>3.4443887749228519E-2</v>
+        <v>3.475941023606554E-2</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
@@ -1848,12 +1854,6 @@
       <c r="B12" s="7"/>
       <c r="C12" s="6">
         <v>5</v>
-      </c>
-      <c r="D12">
-        <v>0.19398709841939801</v>
-      </c>
-      <c r="E12">
-        <v>1.3554534919491065E-2</v>
       </c>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
@@ -1874,16 +1874,16 @@
         <v>1</v>
       </c>
       <c r="D13">
-        <v>1.3990351767510919E-4</v>
+        <v>8.4733626044853011E-4</v>
       </c>
       <c r="E13">
-        <v>6.6863921420714498E-2</v>
+        <v>0.14690428482304824</v>
       </c>
       <c r="F13">
-        <v>1.3569738726230699E-4</v>
+        <v>8.4733626044853011E-4</v>
       </c>
       <c r="G13">
-        <v>6.2395652717977278E-2</v>
+        <v>0.14526614972371041</v>
       </c>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
@@ -1900,16 +1900,16 @@
         <v>2</v>
       </c>
       <c r="D14">
-        <v>5.7969661008387642E-3</v>
+        <v>6.2422531657229056E-3</v>
       </c>
       <c r="E14">
-        <v>0.82987275200412658</v>
+        <v>0.7567534537955708</v>
       </c>
       <c r="F14">
-        <v>5.7969661008387633E-3</v>
+        <v>6.1357258277597148E-3</v>
       </c>
       <c r="G14">
-        <v>0.84221509606098466</v>
+        <v>0.76411398617563442</v>
       </c>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
@@ -1926,16 +1926,16 @@
         <v>3</v>
       </c>
       <c r="D15">
-        <v>0.1665279378791571</v>
+        <v>0.26566231827347758</v>
       </c>
       <c r="E15">
-        <v>9.8558655614783136E-2</v>
+        <v>9.3273023901056004E-2</v>
       </c>
       <c r="F15">
-        <v>0.16652793787915701</v>
+        <v>0.26566231827347758</v>
       </c>
       <c r="G15">
-        <v>0.10092850014657261</v>
+        <v>9.2515079156380478E-2</v>
       </c>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
@@ -1952,10 +1952,10 @@
         <v>4</v>
       </c>
       <c r="D16">
-        <v>0.16152135737471721</v>
+        <v>0.26566231827347758</v>
       </c>
       <c r="E16">
-        <v>8.3709700826493469E-2</v>
+        <v>9.465329387860727E-2</v>
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
@@ -1965,7 +1965,7 @@
       <c r="M16" s="10"/>
       <c r="N16" s="10"/>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1981,7 +1981,7 @@
       <c r="M17" s="10"/>
       <c r="N17" s="10"/>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A19" s="10"/>
       <c r="B19" s="10" t="s">
         <v>6</v>
@@ -1999,7 +1999,7 @@
       <c r="M19" s="10"/>
       <c r="N19" s="10"/>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A20" s="1"/>
       <c r="B20" s="2"/>
       <c r="C20" s="3"/>
@@ -2023,7 +2023,7 @@
       <c r="M20" s="2"/>
       <c r="N20" s="10"/>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A21" s="1"/>
       <c r="B21" s="2"/>
       <c r="C21" s="3" t="s">
@@ -2057,25 +2057,25 @@
       </c>
       <c r="N21" s="10"/>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A22" s="1"/>
       <c r="B22" s="9" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="C22" s="5">
         <v>1</v>
       </c>
       <c r="D22">
-        <v>1.185302047851078E-3</v>
+        <v>1.61099985825943E-3</v>
       </c>
       <c r="E22">
-        <v>0.68685225460181532</v>
+        <v>0.70243247259634778</v>
       </c>
       <c r="F22">
-        <v>1.149666525066006E-3</v>
+        <v>1.1187205415065359E-3</v>
       </c>
       <c r="G22">
-        <v>0.68145767112879718</v>
+        <v>0.62605681373561139</v>
       </c>
       <c r="H22" s="1"/>
       <c r="I22">
@@ -2092,24 +2092,33 @@
         <v>0.6</v>
       </c>
       <c r="N22" s="10"/>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="O22" t="s">
+        <v>19</v>
+      </c>
+      <c r="P22">
+        <v>1.61099985825943E-3</v>
+      </c>
+      <c r="Q22">
+        <v>0.70243247259634778</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A23" s="1"/>
       <c r="B23" s="3"/>
       <c r="C23">
         <v>2</v>
       </c>
       <c r="D23">
-        <v>7.1779561477931936E-3</v>
+        <v>9.635665677864837E-3</v>
       </c>
       <c r="E23">
-        <v>0.2565189652707478</v>
+        <v>0.22545232964853451</v>
       </c>
       <c r="F23">
-        <v>6.9621544284604077E-3</v>
+        <v>6.0291786234855493E-3</v>
       </c>
       <c r="G23">
-        <v>0.28550337400040016</v>
+        <v>0.39744101704231144</v>
       </c>
       <c r="H23" s="1"/>
       <c r="I23">
@@ -2126,24 +2135,30 @@
         <v>0.3</v>
       </c>
       <c r="N23" s="10"/>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="P23">
+        <v>9.635665677864837E-3</v>
+      </c>
+      <c r="Q23">
+        <v>0.22545232964853451</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A24" s="1"/>
       <c r="B24" s="3"/>
       <c r="C24">
         <v>3</v>
       </c>
       <c r="D24">
-        <v>0.13044574444085549</v>
+        <v>0.1497809921024926</v>
       </c>
       <c r="E24">
-        <v>9.2795713745085592E-2</v>
+        <v>9.8309419491559719E-2</v>
       </c>
       <c r="F24">
-        <v>0.138657770471422</v>
+        <v>0.15240468466226989</v>
       </c>
       <c r="G24">
-        <v>0.10371531816949794</v>
+        <v>0.12008145558233596</v>
       </c>
       <c r="H24" s="1"/>
       <c r="I24">
@@ -2160,18 +2175,24 @@
         <v>0.1</v>
       </c>
       <c r="N24" s="10"/>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="P24">
+        <v>0.1497809921024926</v>
+      </c>
+      <c r="Q24">
+        <v>9.8309419491559719E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A25" s="1"/>
       <c r="B25" s="3"/>
       <c r="C25">
         <v>4</v>
       </c>
       <c r="D25">
-        <v>0.16402464762693714</v>
+        <v>0.20474143893734029</v>
       </c>
       <c r="E25">
-        <v>8.5075205497019052E-2</v>
+        <v>8.6955321020121823E-2</v>
       </c>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
@@ -2180,8 +2201,14 @@
       <c r="L25" s="10"/>
       <c r="M25" s="10"/>
       <c r="N25" s="10"/>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="P25">
+        <v>0.20474143893734029</v>
+      </c>
+      <c r="Q25">
+        <v>8.6955321020121823E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A26" s="1"/>
       <c r="B26" s="8" t="s">
         <v>7</v>
@@ -2190,16 +2217,16 @@
         <v>1</v>
       </c>
       <c r="D26">
-        <v>6.8422724049203854E-4</v>
+        <v>1.61099985825943E-3</v>
       </c>
       <c r="E26">
-        <v>0.47221012370451171</v>
+        <v>0.70243247259634778</v>
       </c>
       <c r="F26">
-        <v>1.149666525066006E-3</v>
+        <v>1.1187205415065359E-3</v>
       </c>
       <c r="G26">
-        <v>0.68145767112879718</v>
+        <v>0.62605681373561139</v>
       </c>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
@@ -2208,24 +2235,30 @@
       <c r="L26" s="10"/>
       <c r="M26" s="10"/>
       <c r="N26" s="10"/>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="P26">
+        <v>0.21197711581854251</v>
+      </c>
+      <c r="Q26">
+        <v>6.8839707399211775E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A27" s="1"/>
       <c r="B27" s="2"/>
       <c r="C27">
         <v>2</v>
       </c>
       <c r="D27">
-        <v>4.1435456357150086E-3</v>
+        <v>9.635665677864837E-3</v>
       </c>
       <c r="E27">
-        <v>0.43602579253040996</v>
+        <v>0.22545232964853451</v>
       </c>
       <c r="F27">
-        <v>6.9621544284604077E-3</v>
+        <v>6.0291786234855493E-3</v>
       </c>
       <c r="G27">
-        <v>0.28550337400040016</v>
+        <v>0.39744101704231144</v>
       </c>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
@@ -2235,23 +2268,23 @@
       <c r="M27" s="10"/>
       <c r="N27" s="10"/>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A28" s="1"/>
       <c r="B28" s="2"/>
       <c r="C28">
         <v>3</v>
       </c>
       <c r="D28">
-        <v>5.3823583219442972E-2</v>
+        <v>0.1497809921024926</v>
       </c>
       <c r="E28">
-        <v>9.2190047205541886E-2</v>
+        <v>9.8309419491559719E-2</v>
       </c>
       <c r="F28">
-        <v>0.138657770471422</v>
+        <v>0.15240468466226989</v>
       </c>
       <c r="G28">
-        <v>0.10371531816949794</v>
+        <v>0.12008145558233596</v>
       </c>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
@@ -2261,17 +2294,17 @@
       <c r="M28" s="10"/>
       <c r="N28" s="10"/>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A29" s="1"/>
       <c r="B29" s="2"/>
       <c r="C29">
         <v>4</v>
       </c>
       <c r="D29">
-        <v>0.17168970435252909</v>
+        <v>0.20474143893734029</v>
       </c>
       <c r="E29">
-        <v>6.4267458635436037E-2</v>
+        <v>8.6955321020121823E-2</v>
       </c>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
@@ -2281,17 +2314,17 @@
       <c r="M29" s="10"/>
       <c r="N29" s="10"/>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A30" s="1"/>
       <c r="B30" s="2"/>
       <c r="C30">
         <v>5</v>
       </c>
       <c r="D30">
-        <v>0.19398709841939801</v>
+        <v>0.21197711581854251</v>
       </c>
       <c r="E30">
-        <v>2.243589780687992E-2</v>
+        <v>6.8839707399211775E-2</v>
       </c>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
@@ -2301,17 +2334,11 @@
       <c r="M30" s="10"/>
       <c r="N30" s="10"/>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A31" s="1"/>
       <c r="B31" s="7"/>
       <c r="C31" s="6">
         <v>6</v>
-      </c>
-      <c r="D31">
-        <v>0.19398709841939801</v>
-      </c>
-      <c r="E31">
-        <v>2.097187165219656E-2</v>
       </c>
       <c r="F31" s="6"/>
       <c r="G31" s="6"/>
@@ -2323,7 +2350,7 @@
       <c r="M31" s="10"/>
       <c r="N31" s="10"/>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A32" s="1"/>
       <c r="B32" s="3" t="s">
         <v>3</v>
@@ -2332,16 +2359,16 @@
         <v>1</v>
       </c>
       <c r="D32">
-        <v>2.423579714286543E-4</v>
+        <v>8.7728159746556708E-4</v>
       </c>
       <c r="E32">
-        <v>0.2769056696081883</v>
+        <v>0.58947376395780982</v>
       </c>
       <c r="F32">
-        <v>1.0815773628198939E-3</v>
+        <v>8.7728159746556698E-4</v>
       </c>
       <c r="G32">
-        <v>0.51451800524751246</v>
+        <v>0.58961735864715192</v>
       </c>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
@@ -2358,16 +2385,16 @@
         <v>2</v>
       </c>
       <c r="D33">
-        <v>3.3463555771238722E-3</v>
+        <v>5.2471712739034426E-3</v>
       </c>
       <c r="E33">
-        <v>0.52087720512110969</v>
+        <v>0.28926239543313736</v>
       </c>
       <c r="F33">
-        <v>4.4043966490246791E-3</v>
+        <v>5.2471712739034426E-3</v>
       </c>
       <c r="G33">
-        <v>0.38431596858261574</v>
+        <v>0.28926239543313736</v>
       </c>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
@@ -2384,16 +2411,16 @@
         <v>3</v>
       </c>
       <c r="D34">
-        <v>0.1566652972494203</v>
+        <v>0.2156902891245093</v>
       </c>
       <c r="E34">
-        <v>0.19954395844798126</v>
+        <v>0.11611746062601215</v>
       </c>
       <c r="F34">
-        <v>0.1566652972494203</v>
+        <v>0.2156902891245093</v>
       </c>
       <c r="G34">
-        <v>0.20243427256110791</v>
+        <v>0.11686327110461661</v>
       </c>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
@@ -2410,10 +2437,10 @@
         <v>4</v>
       </c>
       <c r="D35">
-        <v>0.1566652972494203</v>
+        <v>0.26108886143117699</v>
       </c>
       <c r="E35">
-        <v>0.19833030845553501</v>
+        <v>0.10304111241787529</v>
       </c>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>

</xml_diff>